<commit_message>
added code line of priority assesment
</commit_message>
<xml_diff>
--- a/model_description/list_equations_and_linecode.xlsx
+++ b/model_description/list_equations_and_linecode.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abaezaca\Dropbox (ASU)\MEGADAPT\SHV\model_description\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6975"/>
+    <workbookView xWindow="12660" yWindow="-21000" windowWidth="19180" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,8 +26,11 @@
     <definedName name="_Toc496282691" localSheetId="0">Sheet1!$A$37</definedName>
     <definedName name="_Toc496282698" localSheetId="0">Sheet1!$A$46</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="34">
   <si>
     <t>equation</t>
   </si>
@@ -151,12 +149,15 @@
   <si>
     <t>also in setup_template_empirical.xml</t>
   </si>
+  <si>
+    <t>code line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +189,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,8 +223,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -223,7 +244,11 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -282,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,19 +527,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +551,14 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -538,8 +571,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>343</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,13 +593,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4">
         <f t="shared" ref="B4:B40" si="0">B3+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -572,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -587,7 +626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -599,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -614,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -629,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -644,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -659,7 +698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -674,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -689,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -704,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -719,7 +758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -734,7 +773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -749,7 +788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -764,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -779,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -794,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -809,7 +848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -824,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -839,7 +878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -854,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -869,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -884,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -899,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
@@ -914,7 +953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -929,7 +968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16">
       <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
@@ -944,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -959,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16">
       <c r="A32" s="3" t="s">
         <v>25</v>
       </c>
@@ -974,7 +1013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="16">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -989,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="16">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -1004,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="16">
       <c r="A35" s="3" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="16">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -1034,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="16">
       <c r="A37" s="3" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="16">
       <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
@@ -1064,7 +1103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="16">
       <c r="A39" s="3" t="s">
         <v>26</v>
       </c>
@@ -1079,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="16">
       <c r="A40" s="3" t="s">
         <v>26</v>
       </c>
@@ -1094,7 +1133,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="16">
       <c r="A41" s="3" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="16">
       <c r="A42" s="3" t="s">
         <v>26</v>
       </c>
@@ -1122,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="16">
       <c r="A43" s="3" t="s">
         <v>26</v>
       </c>
@@ -1136,7 +1175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="16">
       <c r="A44" s="3" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="16">
       <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
@@ -1164,7 +1203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="16">
       <c r="A46" s="3" t="s">
         <v>31</v>
       </c>
@@ -1181,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="16">
       <c r="A47" s="3" t="s">
         <v>31</v>
       </c>
@@ -1198,7 +1237,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16">
       <c r="A48" s="3" t="s">
         <v>31</v>
       </c>
@@ -1215,7 +1254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="16">
       <c r="A49" s="3" t="s">
         <v>31</v>
       </c>
@@ -1231,6 +1270,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit lines for exposure
</commit_message>
<xml_diff>
--- a/model_description/list_equations_and_linecode.xlsx
+++ b/model_description/list_equations_and_linecode.xlsx
@@ -519,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -620,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -632,7 +632,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>322</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>

</xml_diff>